<commit_message>
EPBDS-11942 add warning for ne. update test
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11942_eq_for_different_types_warnings.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11942_eq_for_different_types_warnings.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="136">
   <si>
     <t>Step</t>
   </si>
@@ -600,6 +600,45 @@
   </si>
   <si>
     <t>=bank2==bank3</t>
+  </si>
+  <si>
+    <t>=bank2!=bank3</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult  Example2 (Bank [] banks, Bank2 bank2, Bank3 bank3)</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult  Example2 (Integer[] intArr1, int[] intArr2, Double[] dArr, Float[] floatArr, int i2, Integer i2, )</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult  Example2 (Integer[] intArr1, int[] intArr2, Double[] dArr, Float[] floatArr, int i2, Integer i2, Double d, float f)</t>
+  </si>
+  <si>
+    <t>=intArr1&gt;i1</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult  Example2 (Integer[] intArr1, int[] intArr2, Double[] dArr, Float[] floatArr, int i1, Integer i2, Double d, float f)</t>
+  </si>
+  <si>
+    <t>=intArr2&lt;i2</t>
+  </si>
+  <si>
+    <t>=dArr&gt;=i1</t>
+  </si>
+  <si>
+    <t>=dArr&gt;=floatArr</t>
+  </si>
+  <si>
+    <t>=dArr&lt;=floatArr</t>
+  </si>
+  <si>
+    <t>=d==f</t>
+  </si>
+  <si>
+    <t>=floatArr&lt;=f</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult  Example2 (Integer[] intArr1, int[] intArr2, Double[] dArr, Float[] floatArr, int i1, Integer i2, float f)</t>
   </si>
 </sst>
 </file>
@@ -1501,7 +1540,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CB6654-7B4F-48C7-9930-3A14DB2CEDF4}">
-  <dimension ref="A3:I51"/>
+  <dimension ref="A3:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
@@ -1578,6 +1617,12 @@
       <c r="A7" t="s">
         <v>89</v>
       </c>
+      <c r="C7" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1747,13 +1792,68 @@
         <v>120</v>
       </c>
     </row>
+    <row r="53">
+      <c r="B53" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="38"/>
+    </row>
+    <row r="54">
+      <c r="B54" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="C54" t="s" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="s" s="14">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s" s="15">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="s" s="14">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s" s="15">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="s" s="14">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s" s="15">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B53:C53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>